<commit_message>
Initial modifications, much to do
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/BHM_Covid_Testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE505EE5-5B78-9946-A0D6-EB0788A70FE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508572B-B91C-D040-9027-E729661C971E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1820" windowWidth="23440" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
+    <workbookView xWindow="1360" yWindow="2180" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +153,13 @@
     <font>
       <sz val="12"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,10 +185,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +507,10 @@
   <dimension ref="A2:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,9 +637,10 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="F4" s="3"/>
       <c r="G4" t="s">
         <v>27</v>
       </c>
@@ -652,7 +661,8 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H5" t="s">

</xml_diff>

<commit_message>
Fixed sensitivity specificity bug. Added plots for false positives and false negatives
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/BHM_Covid_Testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508572B-B91C-D040-9027-E729661C971E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AE4008-9D46-5C40-A1EC-4B6D9AFB45BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="2180" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -142,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +153,13 @@
     <font>
       <sz val="12"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,11 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,12 +518,12 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12:B15"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -571,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -627,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>0</v>
       </c>
@@ -651,7 +659,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1</v>
       </c>
@@ -675,7 +683,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>2</v>
       </c>
@@ -693,7 +701,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>3</v>
       </c>
@@ -711,7 +719,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>4</v>
       </c>
@@ -721,7 +729,7 @@
       <c r="H8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="1"/>
@@ -734,7 +742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>5</v>
       </c>
@@ -744,7 +752,7 @@
       <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K9" s="1"/>
@@ -757,7 +765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>6</v>
       </c>
@@ -772,7 +780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>7</v>
       </c>
@@ -787,7 +795,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>8</v>
       </c>
@@ -797,9 +805,7 @@
       <c r="I12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
         <v>30</v>
@@ -812,16 +818,14 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
         <v>28</v>
       </c>
@@ -837,7 +841,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>10</v>
       </c>
@@ -864,7 +868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>11</v>
       </c>
@@ -891,7 +895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>12</v>
       </c>
@@ -912,7 +916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>13</v>
       </c>
@@ -933,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>14</v>
       </c>
@@ -951,7 +955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>15</v>
       </c>
@@ -969,7 +973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Updated transition matrix documentation .xls
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/BHM_Covid_Testing/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AE4008-9D46-5C40-A1EC-4B6D9AFB45BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35EF3DBF-BB63-1041-979A-CEE6122535B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="2180" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
@@ -24,8 +24,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B925A70B-340C-9A4B-A632-1BB572207AC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>release rate for asymptomatic positives</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{E81BAEA6-2C62-3F43-9C91-3D1FC1270860}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>release rate for asymptomatic positives</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -136,13 +212,16 @@
   </si>
   <si>
     <t>gamma*labda*alpha_t</t>
+  </si>
+  <si>
+    <t>r^AP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,13 +250,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,12 +290,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,14 +610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4172083D-8402-E94E-8719-CF901282B3C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4172083D-8402-E94E-8719-CF901282B3C7}">
   <dimension ref="A2:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -787,6 +886,9 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -824,6 +926,9 @@
       </c>
       <c r="B13" t="s">
         <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
@@ -987,5 +1092,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed falsed negative transitions: cannot go to recovered or dead straight from this state
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35EF3DBF-BB63-1041-979A-CEE6122535B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B72E5AD-2EFD-3B4F-8658-538F70E55FAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="2180" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -617,7 +617,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -965,13 +965,9 @@
         <v>29</v>
       </c>
       <c r="P14" s="2"/>
-      <c r="Q14" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15">
@@ -993,12 +989,8 @@
         <v>29</v>
       </c>
       <c r="Q15" s="2"/>
-      <c r="R15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16">

</xml_diff>

<commit_message>
Include sensitivity into transitions from known not infected asymptomatic to known infected asymptomatic (both NQ and Q). Without this (or some other modification) these transitions would happen with implicit 100% sensitivity.
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B72E5AD-2EFD-3B4F-8658-538F70E55FAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D7A92-DE92-9143-9403-3FB75CAAB89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2180" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
+    <workbookView xWindow="100" yWindow="2400" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,39 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{8F3A9828-2D04-9A45-9E0C-64F1F70C9441}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sensitivity added to account for reduced knowledge in transitions from known not infected to known infected. Without this, the structure would imply perfect sensitivity for these transitions.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B925A70B-340C-9A4B-A632-1BB572207AC2}">
       <text>
         <r>
@@ -101,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -215,6 +248,18 @@
   </si>
   <si>
     <t>r^AP</t>
+  </si>
+  <si>
+    <t>labda*alpha_t*sens</t>
+  </si>
+  <si>
+    <t>labda*alpha_t*(1-sens)</t>
+  </si>
+  <si>
+    <t>labda^Q*alpha_t*sens</t>
+  </si>
+  <si>
+    <t>labda^Q*alpha_t*(1-sens)</t>
   </si>
 </sst>
 </file>
@@ -617,7 +662,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -792,12 +837,13 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="1"/>
+      <c r="I6" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:19">
@@ -810,13 +856,14 @@
       <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" t="s">
-        <v>28</v>
+      <c r="J7" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">

</xml_diff>

<commit_message>
Add transitions from known to unknown not infected (both nQ and Q). Add try-except for initial population in optimizer.
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D7A92-DE92-9143-9403-3FB75CAAB89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D75B38-FD87-6B4D-8CD2-C8C7C2CF8B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="2400" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>labda^Q*alpha_t*(1-sens)</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>sigma^Q</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -834,6 +840,9 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
@@ -852,6 +861,9 @@
       </c>
       <c r="B7" t="s">
         <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Updated transition matrix: 1) Added test and trace effects 2) modified transitions from known uninfected states so that those who are infected transition to unknown infected (infection rate) or back to unknown not infected (sigma). Removed transitions from known not infected to known unfected. Trials on running on Triton -> check results.
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C142127-4728-B342-A699-82E4F63430EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00036C41-3614-844A-BA5D-3CF20470B793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="2400" windowWidth="25280" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
+    <workbookView xWindow="6740" yWindow="1220" windowWidth="23340" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B925A70B-340C-9A4B-A632-1BB572207AC2}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{048E8170-A4A6-BC4D-8A90-B891A50E393A}">
       <text>
         <r>
           <rPr>
@@ -92,11 +92,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>release rate for asymptomatic positives</t>
+          <t>Should these be retested and unquarantined in case of false negative?</t>
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{E81BAEA6-2C62-3F43-9C91-3D1FC1270860}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{E81BAEA6-2C62-3F43-9C91-3D1FC1270860}">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>release rate for asymptomatic positives</t>
+          <t>retesting rate for asymptomatic positives</t>
         </r>
       </text>
     </comment>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>NA, NQ</t>
   </si>
@@ -199,27 +199,12 @@
     <t>ksi^u</t>
   </si>
   <si>
-    <t>tau*sens</t>
-  </si>
-  <si>
-    <t>tau*(1-sens)</t>
-  </si>
-  <si>
-    <t>tau*spec</t>
-  </si>
-  <si>
-    <t>tau*(1-spec)</t>
-  </si>
-  <si>
     <t>ksi^-</t>
   </si>
   <si>
     <t>r^-</t>
   </si>
   <si>
-    <t>labda*alpha_t</t>
-  </si>
-  <si>
     <t>labda^Q*alpha_t</t>
   </si>
   <si>
@@ -244,28 +229,46 @@
     <t>r^r</t>
   </si>
   <si>
-    <t>gamma*labda*alpha_t</t>
-  </si>
-  <si>
-    <t>r^AP</t>
-  </si>
-  <si>
-    <t>labda*alpha_t*sens</t>
-  </si>
-  <si>
-    <t>labda*alpha_t*(1-sens)</t>
-  </si>
-  <si>
-    <t>labda^Q*alpha_t*sens</t>
-  </si>
-  <si>
-    <t>labda^Q*alpha_t*(1-sens)</t>
-  </si>
-  <si>
     <t>sigma</t>
   </si>
   <si>
     <t>sigma^Q</t>
+  </si>
+  <si>
+    <t>lockdown_eff*lambda*alpha_t</t>
+  </si>
+  <si>
+    <t>lambda^Q*alpha_t</t>
+  </si>
+  <si>
+    <t>tau_re^AP*test_spec</t>
+  </si>
+  <si>
+    <t>gamma*lockdown_eff*lambda*alpha_t</t>
+  </si>
+  <si>
+    <t>tau*(1-spec) + tau_TT^NQ*(1-spec)</t>
+  </si>
+  <si>
+    <t>tau*spec + tau_TT^NQ*spec</t>
+  </si>
+  <si>
+    <t>tau*spec +  tau_TT^Q*spec</t>
+  </si>
+  <si>
+    <t>tau*(1-spec)+ tau_TT^Q*(1-spec)</t>
+  </si>
+  <si>
+    <t>tau*sens + tau_TT^NQ*sens</t>
+  </si>
+  <si>
+    <t>tau*sens + tau_TT^Q*sens</t>
+  </si>
+  <si>
+    <t>tau*(1-sens) + tau_TT^Q*(1-sens)</t>
+  </si>
+  <si>
+    <t>tau*(1-sens) +  tau_TT^NQ*(1-sens)</t>
   </si>
 </sst>
 </file>
@@ -341,13 +344,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +672,15 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
@@ -796,14 +805,14 @@
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -821,14 +830,14 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -841,18 +850,17 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="5"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="M6" s="5"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:19">
@@ -863,19 +871,18 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="5"/>
       <c r="K7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">
@@ -888,16 +895,16 @@
         <v>20</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -911,16 +918,16 @@
         <v>19</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="P9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -929,13 +936,16 @@
       </c>
       <c r="B10" t="s">
         <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -945,15 +955,13 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="J11" s="6"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="P11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -964,12 +972,12 @@
         <v>13</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -986,15 +994,15 @@
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
+      <c r="F13" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1018,10 +1026,10 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1040,12 +1048,12 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1063,13 +1071,13 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="P16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Q16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1084,13 +1092,13 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="R17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="S17" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -1108,7 +1116,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="R18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -1126,7 +1134,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="Q19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:19">

</xml_diff>

<commit_message>
Implements rough draft of test and trace. Next: update whole epidemic model to final_v1 :)
</commit_message>
<xml_diff>
--- a/documentation/transition_matrix_w_sens_spec.xlsx
+++ b/documentation/transition_matrix_w_sens_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljneuvon/Work/Epidemic control/Covid_policies_w_imperfect_testing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00036C41-3614-844A-BA5D-3CF20470B793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF36322-055D-ED4E-B8CB-3DF8614243B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="1220" windowWidth="23340" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
+    <workbookView xWindow="22520" yWindow="13320" windowWidth="23340" windowHeight="14840" xr2:uid="{59EEBB9C-DF2A-EC4F-BD0B-CDAFEE3749BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>